<commit_message>
redact ExcelHelper.java file for add default fields in excel files(userid, product name and act)
</commit_message>
<xml_diff>
--- a/src/main/resources/data/orders.xlsx
+++ b/src/main/resources/data/orders.xlsx
@@ -12,7 +12,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,12 +71,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.9453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.859375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.49609375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>